<commit_message>
Ended session, todo left inside
</commit_message>
<xml_diff>
--- a/Dokumentation/Sprint02.xlsx
+++ b/Dokumentation/Sprint02.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Krav</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Undersöka iOS Developer Program och eventuellt ansöka</t>
+  </si>
+  <si>
+    <t>Jobba med Player-class (poängräkning, positionering med mera)</t>
+  </si>
+  <si>
+    <t>Påbörjad</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
   <dimension ref="A2:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -530,13 +536,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -547,13 +553,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -628,11 +634,14 @@
       <c r="A11">
         <v>14</v>
       </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -644,11 +653,11 @@
       </c>
       <c r="E13">
         <f>SUM(E5:E12)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F13">
         <f>SUM(F5:F11)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6">

</xml_diff>

<commit_message>
Fixed ball-problem plus score is counting
</commit_message>
<xml_diff>
--- a/Dokumentation/Sprint02.xlsx
+++ b/Dokumentation/Sprint02.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Krav</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Påbörjad</t>
+  </si>
+  <si>
+    <t>Slutförd</t>
   </si>
 </sst>
 </file>
@@ -115,12 +118,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -153,13 +162,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +504,7 @@
   <dimension ref="A2:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -536,13 +546,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -553,7 +563,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -570,17 +580,17 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>11</v>
       </c>
       <c r="C8" t="s">
@@ -597,7 +607,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>12</v>
       </c>
       <c r="C9" t="s">
@@ -621,13 +631,13 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -644,20 +654,25 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="D15" t="s">
         <v>5</v>
       </c>
-      <c r="E13">
-        <f>SUM(E5:E12)</f>
+      <c r="E15">
+        <f>SUM(E5:E13)</f>
         <v>21</v>
       </c>
-      <c r="F13">
-        <f>SUM(F5:F11)</f>
-        <v>3</v>
+      <c r="F15">
+        <f>SUM(F5:F13)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6">

</xml_diff>